<commit_message>
Commit Problemas básicos solucionados
</commit_message>
<xml_diff>
--- a/resources/usuarios.xlsx
+++ b/resources/usuarios.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>123</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>navichoque</t>
+  </si>
+  <si>
+    <t>dnavichoque@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B5FB0C-BAF5-4F53-947E-584373B9FB86}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -532,6 +538,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit resolver problemas de codigos y contraseñas
</commit_message>
<xml_diff>
--- a/resources/usuarios.xlsx
+++ b/resources/usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mynit\OneDrive\Escritorio\POO\ProyectoMynorBarrriosAndreGil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mynit\OneDrive\Escritorio\POO\costeoRapido\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F8D40A-FCBA-4B11-B81A-FE31F36149FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D79B6DD-C69A-4783-BDDB-99E4D2A51D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1575" windowWidth="15375" windowHeight="7785" xr2:uid="{8DBC6ABC-22F8-458A-B29D-8655618A5079}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8DBC6ABC-22F8-458A-B29D-8655618A5079}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
-  <si>
-    <t>123</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>mynor</t>
   </si>
@@ -74,9 +71,6 @@
     <t>meme@gmail.com</t>
   </si>
   <si>
-    <t>1234</t>
-  </si>
-  <si>
     <t>navichoque</t>
   </si>
   <si>
@@ -95,7 +89,16 @@
     <t>andregil003@gmail.com</t>
   </si>
   <si>
-    <t>mynorxd</t>
+    <t>mynor3</t>
+  </si>
+  <si>
+    <t>barriosmynitor@gmail.com</t>
+  </si>
+  <si>
+    <t>Mynor123!</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -103,8 +106,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -153,9 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,100 +502,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B5FB0C-BAF5-4F53-947E-584373B9FB86}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+      <c r="B3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+      <c r="B4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+      <c r="B5" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="C5" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="B6" t="s" s="0">
         <v>12</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+      <c r="C6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B7" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C6" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+      <c r="C7" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C7" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+      <c r="C8" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B9" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>12</v>
+      <c r="C9" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit corrección errores y FAQ parte 1
</commit_message>
<xml_diff>
--- a/resources/usuarios.xlsx
+++ b/resources/usuarios.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>mynor</t>
   </si>
@@ -640,7 +640,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit eliminar boton innecesario
</commit_message>
<xml_diff>
--- a/resources/usuarios.xlsx
+++ b/resources/usuarios.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>mynor</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t>josegc2910@gmail.com</t>
+  </si>
+  <si>
+    <t>Dani</t>
+  </si>
+  <si>
+    <t>ellydanielabc@gmail.com</t>
+  </si>
+  <si>
+    <t>Dani_</t>
+  </si>
+  <si>
+    <t>dani@gmail.com</t>
+  </si>
+  <si>
+    <t>Dani_1</t>
+  </si>
+  <si>
+    <t>danibc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -543,7 +561,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B5FB0C-BAF5-4F53-947E-584373B9FB86}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -643,6 +661,39 @@
         <v>19</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{99262334-F08A-4B7C-B439-06F3B411088D}"/>

</xml_diff>